<commit_message>
End of 5th semester
</commit_message>
<xml_diff>
--- a/Others/bonus_list.xlsx
+++ b/Others/bonus_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>student_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>bonus_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bonus_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bonus_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bonus_4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,20 +560,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="19.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,152 +584,205 @@
       <c r="C1" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>5140309478</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>5140309479</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>5140309480</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>5140309481</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5140309482</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5140309484</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5140309485</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>5140309487</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>5140309488</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>5140309489</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>5140309491</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>5140309493</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>5140309494</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>5140309495</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>5140309496</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>5140309497</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5140309498</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>5140309499</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>5140309500</v>
       </c>
@@ -726,16 +792,25 @@
       <c r="C20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>5140309502</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>5140309503</v>
       </c>
@@ -745,24 +820,32 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>5140309504</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>5140309505</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>5140309507</v>
       </c>
@@ -772,24 +855,32 @@
       <c r="C25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>5140309508</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>5140309509</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>5140309510</v>
       </c>
@@ -799,32 +890,41 @@
       <c r="C28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>5140309511</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>5140309512</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>5140309513</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>5140309514</v>
       </c>
@@ -834,200 +934,249 @@
       <c r="C32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>5140309515</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>5140309516</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>5140309517</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>5140309518</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>5140309519</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>5140309520</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>5140309521</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>5140309523</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>5140309524</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>5140309525</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>5140309526</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>5140309527</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>5140309528</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>5140309529</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>5140309530</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>5140309531</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>5140309532</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>5140309533</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>5140309534</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>5140309535</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>5140309537</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>5140309539</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>5140309541</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>5140309542</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>5140309543</v>
       </c>
@@ -1037,30 +1186,39 @@
       <c r="C57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>5140309545</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>5140309546</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>5140309547</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="F60" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>